<commit_message>
Surveys + updated bug report
First lot of surveys + updated bug report with initial results.
</commit_message>
<xml_diff>
--- a/Bug Report.xlsx
+++ b/Bug Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="2780" yWindow="460" windowWidth="29440" windowHeight="18980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>Bug Reported</t>
   </si>
@@ -39,13 +39,160 @@
   </si>
   <si>
     <t>Number of Reports</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Non Bugs</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Lag at end of round</t>
+  </si>
+  <si>
+    <t>User reported a few seconds of lag at end of each round</t>
+  </si>
+  <si>
+    <t>1 (001)</t>
+  </si>
+  <si>
+    <t>Logout cant log back in</t>
+  </si>
+  <si>
+    <t>If a user logged out, they could see all fields on the log in screen, none of them worked</t>
+  </si>
+  <si>
+    <t>White in Lobby</t>
+  </si>
+  <si>
+    <t>User did not know what white meant in the Game Lobby</t>
+  </si>
+  <si>
+    <t>More feedback in result screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User asks for more types of feedback in results screen, how many questions they get right or wrong. </t>
+  </si>
+  <si>
+    <t>Leaderboard refresh</t>
+  </si>
+  <si>
+    <t>User had to quit app and restart for leaderbaords to update</t>
+  </si>
+  <si>
+    <t>No push notifications</t>
+  </si>
+  <si>
+    <t>Users reported not receving any push notificaitons during testing</t>
+  </si>
+  <si>
+    <t>Cant login with Facebook</t>
+  </si>
+  <si>
+    <t>User could not log in using Facebook</t>
+  </si>
+  <si>
+    <t>Marvel spelt wring</t>
+  </si>
+  <si>
+    <t>Category 'Marvel' is spelt wrong</t>
+  </si>
+  <si>
+    <t>User could not understand Game Lobby</t>
+  </si>
+  <si>
+    <t>1 (002)</t>
+  </si>
+  <si>
+    <t>user was confused as to what each colour meant</t>
+  </si>
+  <si>
+    <t>long questions</t>
+  </si>
+  <si>
+    <t>User spent too much time reading questions rather than answering them</t>
+  </si>
+  <si>
+    <t>Back button login</t>
+  </si>
+  <si>
+    <t>No back button on login screen</t>
+  </si>
+  <si>
+    <t>1 (004)</t>
+  </si>
+  <si>
+    <t>3 (002, 003, 004)</t>
+  </si>
+  <si>
+    <t>Question Submission</t>
+  </si>
+  <si>
+    <t>User not sure if there question was received</t>
+  </si>
+  <si>
+    <t>4 (001, 002, 003, 004)</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>No of Reports: 4</t>
+  </si>
+  <si>
+    <t>Breakdown:</t>
+  </si>
+  <si>
+    <t>Device: 4 Android</t>
+  </si>
+  <si>
+    <t>Gender: 2 male, 2 female</t>
+  </si>
+  <si>
+    <t>Age: 19, 19, 25, 30</t>
+  </si>
+  <si>
+    <t>Averages:</t>
+  </si>
+  <si>
+    <t>User Experience: 7</t>
+  </si>
+  <si>
+    <t>Enjoyment 7.5</t>
+  </si>
+  <si>
+    <t>Login: 5.5</t>
+  </si>
+  <si>
+    <t>gameScene: 6.5</t>
+  </si>
+  <si>
+    <t>Results: 7.5</t>
+  </si>
+  <si>
+    <t>Leaderboards: 6.5</t>
+  </si>
+  <si>
+    <t>Question Submission: 6.5</t>
+  </si>
+  <si>
+    <t>Push Notifications: 4</t>
+  </si>
+  <si>
+    <t>Desgin: 6</t>
+  </si>
+  <si>
+    <t>question Submission: 6.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -56,6 +203,21 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -132,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -143,6 +305,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,29 +599,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="112" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="2" max="2" width="47.83203125" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
+    <row r="1" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -482,14 +667,22 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+    <row r="3" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -501,222 +694,373 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+    <row r="4" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+    <row r="5" spans="1:17" ht="33" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
+      <c r="G5" s="18" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
+      <c r="G10" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
+    <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="A34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>